<commit_message>
update ecc assertion names and correct the ecc assertion names in the xsecure vplan
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\group_vplans\xsecure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE0231-305F-4A66-A280-E3F1C0101FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E88BABB-1FF5-4068-BBD2-2FB75D0E6418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -777,9 +777,6 @@
     <t>A: a_xsecure_rf_ecc_gpr_reset_value, a_xsecure_rf_ecc_gpr_reset_value_rvfi_rs1, a_xsecure_rf_ecc_gpr_reset_value_rvfi_rs2</t>
   </si>
   <si>
-    <t>A: a_xsecure_rf_ecc_gpr_0_syndrome_not_0, a_xsecure_rf_ecc_syndrome_0_gpr_not_0, a_xsecure_rf_ecc_gpr_1_syndrome_not_1, a_xsecure_rf_ecc_syndrome_1_gpr_not_1, a_glitch_xsecure_rf_ecc_gpr_0_syndrom_0, a_glitch_xsecure_rf_ecc_gpr_1_syndrom_1</t>
-  </si>
-  <si>
     <t>A: a_glitch_xsecure_rf_ecc_rs1_bit_fault, a_glitch_xsecure_rf_ecc_rs2_bit_fault</t>
   </si>
   <si>
@@ -1100,12 +1097,15 @@
     <t>A: a_xsecure_hardened_csr_mcause
 A: a_glitch_xsecure_hardened_csr_mismatch_mcause</t>
   </si>
+  <si>
+    <t>A: a_xsecure_rf_ecc_gpr_not_all_0s_or_1s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1631,30 +1631,30 @@
   <dimension ref="A1:Z177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" customWidth="1"/>
-    <col min="5" max="5" width="36.1796875" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" customWidth="1"/>
-    <col min="8" max="8" width="26.1796875" customWidth="1"/>
-    <col min="9" max="9" width="104.453125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="104.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.54296875" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" customWidth="1"/>
-    <col min="18" max="18" width="17.54296875" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="6" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1683,9 +1683,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="238.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="238.5" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>9</v>
@@ -1712,7 +1712,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="150.75" customHeight="1">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
       <c r="C3" s="14" t="s">
@@ -1737,7 +1737,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="117" customHeight="1">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="14" t="s">
@@ -1762,7 +1762,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="90.75" customHeight="1">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="14" t="s">
@@ -1787,7 +1787,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="89.25" customHeight="1" thickBot="1">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="14" t="s">
@@ -1812,7 +1812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="63" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="63" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="16"/>
       <c r="B7" s="18" t="s">
         <v>21</v>
@@ -1839,7 +1839,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="58.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="58.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="16"/>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
@@ -1864,7 +1864,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="90" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="16"/>
       <c r="B9" s="19"/>
       <c r="C9" s="14" t="s">
@@ -1889,7 +1889,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="54.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="54.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="16"/>
       <c r="B10" s="19"/>
       <c r="C10" s="14" t="s">
@@ -1914,7 +1914,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="71.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="71.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="16"/>
       <c r="B11" s="19"/>
       <c r="C11" s="14" t="s">
@@ -1939,7 +1939,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="98.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="98.25" customHeight="1" thickTop="1">
       <c r="A12" s="16"/>
       <c r="B12" s="17" t="s">
         <v>39</v>
@@ -1964,7 +1964,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="81" customHeight="1">
       <c r="A13" s="16"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
@@ -1986,10 +1986,10 @@
         <v>121</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="75.75" customHeight="1">
       <c r="A14" s="16"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14" t="s">
@@ -2011,10 +2011,10 @@
         <v>13</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="108.75" customHeight="1">
       <c r="A15" s="16"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14" t="s">
@@ -2024,7 +2024,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>60</v>
@@ -2036,10 +2036,10 @@
         <v>13</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="48" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
@@ -2064,7 +2064,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="67.5" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
@@ -2086,10 +2086,10 @@
         <v>13</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="67.5" customHeight="1">
       <c r="A18" s="16"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14" t="s">
@@ -2111,10 +2111,10 @@
         <v>37</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="117" customHeight="1">
       <c r="A19" s="16"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
@@ -2124,7 +2124,7 @@
         <v>57</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>60</v>
@@ -2136,10 +2136,10 @@
         <v>36</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="77.25" customHeight="1">
       <c r="A20" s="16"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
@@ -2161,10 +2161,10 @@
         <v>13</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="98.25" customHeight="1">
       <c r="A21" s="16"/>
       <c r="B21" s="13"/>
       <c r="C21" s="14" t="s">
@@ -2174,7 +2174,7 @@
         <v>61</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>60</v>
@@ -2186,10 +2186,10 @@
         <v>36</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="81.75" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="13"/>
       <c r="C22" s="14" t="s">
@@ -2211,10 +2211,10 @@
         <v>13</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="48.75" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14" t="s">
@@ -2236,10 +2236,10 @@
         <v>13</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="50.25" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="14" t="s">
@@ -2261,10 +2261,10 @@
         <v>13</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="51.75" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14" t="s">
@@ -2286,10 +2286,10 @@
         <v>128</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="48.75" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14" t="s">
@@ -2311,10 +2311,10 @@
         <v>13</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="42.5" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="43.5">
       <c r="A27" s="16"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14" t="s">
@@ -2336,10 +2336,10 @@
         <v>36</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="54" customHeight="1">
       <c r="A28" s="16"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14" t="s">
@@ -2364,7 +2364,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="87" customHeight="1">
       <c r="A29" s="16"/>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
@@ -2386,10 +2386,10 @@
         <v>13</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="84" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
@@ -2411,10 +2411,10 @@
         <v>13</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="110.25" customHeight="1" thickBot="1">
       <c r="A31" s="16"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14" t="s">
@@ -2439,7 +2439,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="45" thickTop="1" thickBot="1">
       <c r="A32" s="16"/>
       <c r="B32" s="18" t="s">
         <v>75</v>
@@ -2463,10 +2463,10 @@
         <v>37</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="29.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
       <c r="A33" s="16"/>
       <c r="B33" s="18"/>
       <c r="C33" s="14" t="s">
@@ -2491,7 +2491,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="135.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="135.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A34" s="16"/>
       <c r="B34" s="18"/>
       <c r="C34" s="14" t="s">
@@ -2516,7 +2516,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="67.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" ht="67.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A35" s="16"/>
       <c r="B35" s="18"/>
       <c r="C35" s="14"/>
@@ -2536,10 +2536,10 @@
         <v>37</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="16"/>
       <c r="B36" s="18"/>
       <c r="C36" s="14"/>
@@ -2559,10 +2559,10 @@
         <v>36</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="77.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A37" s="16"/>
       <c r="B37" s="18"/>
       <c r="C37" s="14"/>
@@ -2582,10 +2582,10 @@
         <v>13</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="107.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="107.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A38" s="16"/>
       <c r="B38" s="18"/>
       <c r="C38" s="14"/>
@@ -2593,7 +2593,7 @@
         <v>61</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F38" s="15" t="s">
         <v>60</v>
@@ -2605,10 +2605,10 @@
         <v>37</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="81.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="81.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A39" s="16"/>
       <c r="B39" s="18"/>
       <c r="C39" s="14"/>
@@ -2628,10 +2628,10 @@
         <v>13</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="48.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A40" s="12"/>
       <c r="B40" s="18"/>
       <c r="C40" s="14"/>
@@ -2651,10 +2651,10 @@
         <v>13</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A41" s="12"/>
       <c r="B41" s="18"/>
       <c r="C41" s="14"/>
@@ -2674,10 +2674,10 @@
         <v>13</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A42" s="12"/>
       <c r="B42" s="18"/>
       <c r="C42" s="14" t="s">
@@ -2702,7 +2702,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="110.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="110.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A43" s="16"/>
       <c r="B43" s="18"/>
       <c r="C43" s="14" t="s">
@@ -2727,7 +2727,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="59.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="59.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="16"/>
       <c r="B44" s="18"/>
       <c r="C44" s="14" t="s">
@@ -2752,7 +2752,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="29" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="30" thickTop="1">
       <c r="A45" s="16"/>
       <c r="B45" s="13" t="s">
         <v>85</v>
@@ -2779,7 +2779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="98.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="86.25">
       <c r="A46" s="16"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14" t="s">
@@ -2801,10 +2801,10 @@
         <v>13</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="84.5" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="72">
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14" t="s">
@@ -2829,7 +2829,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="60" customHeight="1">
       <c r="A48" s="16"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14" t="s">
@@ -2854,7 +2854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="132.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="132.75" customHeight="1" thickBot="1">
       <c r="A49" s="16"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14" t="s">
@@ -2876,10 +2876,10 @@
         <v>13</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="203.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="203.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A50" s="16"/>
       <c r="B50" s="18" t="s">
         <v>91</v>
@@ -2903,10 +2903,10 @@
         <v>13</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="102.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="102.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A51" s="16"/>
       <c r="B51" s="18"/>
       <c r="C51" s="14" t="s">
@@ -2928,10 +2928,10 @@
         <v>13</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="29.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="30.75" thickTop="1" thickBot="1">
       <c r="A52" s="16"/>
       <c r="B52" s="18"/>
       <c r="C52" s="14" t="s">
@@ -2956,7 +2956,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="200.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" ht="200.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A53" s="16"/>
       <c r="B53" s="18"/>
       <c r="C53" s="14" t="s">
@@ -2978,10 +2978,10 @@
         <v>13</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="71" thickTop="1" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="72.75" thickTop="1">
       <c r="A54" s="16"/>
       <c r="B54" s="13" t="s">
         <v>94</v>
@@ -3008,17 +3008,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="57.75">
       <c r="A55" s="16"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>11</v>
@@ -3030,20 +3030,20 @@
         <v>13</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="57.75">
       <c r="A56" s="16"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F56" s="15" t="s">
         <v>11</v>
@@ -3055,20 +3055,20 @@
         <v>13</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="57.75">
       <c r="A57" s="16"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F57" s="15" t="s">
         <v>11</v>
@@ -3080,20 +3080,20 @@
         <v>13</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="57.75">
       <c r="A58" s="16"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>11</v>
@@ -3105,21 +3105,21 @@
         <v>13</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J58" s="15"/>
     </row>
-    <row r="59" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="57.75">
       <c r="A59" s="16"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F59" s="15" t="s">
         <v>11</v>
@@ -3131,20 +3131,20 @@
         <v>13</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.75">
       <c r="A60" s="16"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F60" s="15" t="s">
         <v>11</v>
@@ -3156,20 +3156,20 @@
         <v>13</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="57.75">
       <c r="A61" s="16"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F61" s="15" t="s">
         <v>11</v>
@@ -3181,20 +3181,20 @@
         <v>13</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="57.75">
       <c r="A62" s="16"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F62" s="15" t="s">
         <v>11</v>
@@ -3206,20 +3206,20 @@
         <v>13</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="57.75">
       <c r="A63" s="16"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>11</v>
@@ -3231,20 +3231,20 @@
         <v>13</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="57.75">
       <c r="A64" s="16"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>11</v>
@@ -3256,21 +3256,21 @@
         <v>13</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="57.75">
       <c r="A65" s="16"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>11</v>
@@ -3282,21 +3282,21 @@
         <v>13</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="57.75">
       <c r="A66" s="16"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>11</v>
@@ -3308,20 +3308,20 @@
         <v>13</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="57.75">
       <c r="A67" s="16"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>11</v>
@@ -3333,20 +3333,20 @@
         <v>13</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="57.75">
       <c r="A68" s="16"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F68" s="15" t="s">
         <v>11</v>
@@ -3358,20 +3358,20 @@
         <v>13</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="57.75">
       <c r="A69" s="16"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F69" s="15" t="s">
         <v>11</v>
@@ -3383,20 +3383,20 @@
         <v>13</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="57.75">
       <c r="A70" s="16"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F70" s="15" t="s">
         <v>11</v>
@@ -3408,20 +3408,20 @@
         <v>13</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="57.75">
       <c r="A71" s="16"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F71" s="15" t="s">
         <v>11</v>
@@ -3433,20 +3433,20 @@
         <v>13</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="56.5" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="57.75">
       <c r="A72" s="16"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>11</v>
@@ -3458,20 +3458,20 @@
         <v>13</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="57" thickBot="1" x14ac:dyDescent="0.4">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="58.5" thickBot="1">
       <c r="A73" s="16"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>11</v>
@@ -3483,10 +3483,10 @@
         <v>13</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" ht="108.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="1" customFormat="1" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A74" s="12"/>
       <c r="B74" s="18" t="s">
         <v>202</v>
@@ -3510,10 +3510,10 @@
         <v>13</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" ht="29.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="1" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
       <c r="A75" s="12"/>
       <c r="B75" s="18"/>
       <c r="C75" s="14" t="s">
@@ -3535,10 +3535,10 @@
         <v>13</v>
       </c>
       <c r="I75" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="1" customFormat="1" ht="45" thickTop="1" thickBot="1">
       <c r="A76" s="12"/>
       <c r="B76" s="18"/>
       <c r="C76" s="14" t="s">
@@ -3560,10 +3560,10 @@
         <v>13</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="71.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A77" s="12"/>
       <c r="B77" s="18"/>
       <c r="C77" s="14" t="s">
@@ -3585,10 +3585,10 @@
         <v>13</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="71.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A78" s="12"/>
       <c r="B78" s="18"/>
       <c r="C78" s="14" t="s">
@@ -3610,10 +3610,10 @@
         <v>13</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" ht="57.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A79" s="12"/>
       <c r="B79" s="18"/>
       <c r="C79" s="14" t="s">
@@ -3635,10 +3635,10 @@
         <v>13</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="1" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A80" s="12"/>
       <c r="B80" s="18"/>
       <c r="C80" s="16" t="s">
@@ -3648,7 +3648,7 @@
         <v>176</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F80" s="15" t="s">
         <v>120</v>
@@ -3660,10 +3660,10 @@
         <v>13</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" s="1" customFormat="1" ht="101.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="1" customFormat="1" ht="101.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A81" s="12"/>
       <c r="B81" s="18"/>
       <c r="C81" s="14" t="s">
@@ -3685,10 +3685,10 @@
         <v>13</v>
       </c>
       <c r="I81" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="1" customFormat="1" ht="99.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="1" customFormat="1" ht="102" thickTop="1" thickBot="1">
       <c r="A82" s="12"/>
       <c r="B82" s="18"/>
       <c r="C82" s="14" t="s">
@@ -3710,10 +3710,10 @@
         <v>13</v>
       </c>
       <c r="I82" s="16" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="1" customFormat="1" ht="164.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="1" customFormat="1" ht="164.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A83" s="12"/>
       <c r="B83" s="18"/>
       <c r="C83" s="14" t="s">
@@ -3735,10 +3735,10 @@
         <v>13</v>
       </c>
       <c r="I83" s="12" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="1" customFormat="1" ht="85.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A84" s="12"/>
       <c r="B84" s="18"/>
       <c r="C84" s="16" t="s">
@@ -3760,10 +3760,10 @@
         <v>13</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A85" s="12"/>
       <c r="B85" s="18"/>
       <c r="C85" s="16" t="s">
@@ -3785,10 +3785,10 @@
         <v>13</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="1" customFormat="1" ht="57.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A86" s="12"/>
       <c r="B86" s="18"/>
       <c r="C86" s="16" t="s">
@@ -3798,7 +3798,7 @@
         <v>189</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F86" s="15" t="s">
         <v>11</v>
@@ -3810,10 +3810,10 @@
         <v>13</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="1" customFormat="1" ht="57.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A87" s="12"/>
       <c r="B87" s="18"/>
       <c r="C87" s="16" t="s">
@@ -3835,10 +3835,10 @@
         <v>13</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="1" customFormat="1" ht="71.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A88" s="12"/>
       <c r="B88" s="18"/>
       <c r="C88" s="16" t="s">
@@ -3860,10 +3860,10 @@
         <v>13</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="1" customFormat="1" ht="93" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="1" customFormat="1" ht="93" customHeight="1" thickTop="1" thickBot="1">
       <c r="A89" s="12"/>
       <c r="B89" s="18"/>
       <c r="C89" s="16" t="s">
@@ -3885,10 +3885,10 @@
         <v>37</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="98.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="98.25" customHeight="1" thickTop="1">
       <c r="A90" s="16"/>
       <c r="B90" s="13" t="s">
         <v>110</v>
@@ -3912,10 +3912,10 @@
         <v>13</v>
       </c>
       <c r="I90" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="96.75" customHeight="1">
       <c r="A91" s="16"/>
       <c r="B91" s="13"/>
       <c r="C91" s="14" t="s">
@@ -3937,10 +3937,10 @@
         <v>13</v>
       </c>
       <c r="I91" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="95.25" customHeight="1">
       <c r="A92" s="16" t="s">
         <v>203</v>
       </c>
@@ -3964,14 +3964,14 @@
         <v>13</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="99" customHeight="1">
       <c r="A93" s="16"/>
       <c r="B93" s="13"/>
       <c r="C93" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D93" s="15" t="s">
         <v>209</v>
@@ -3989,14 +3989,14 @@
         <v>13</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="81" customHeight="1" thickBot="1">
       <c r="A94" s="16"/>
       <c r="B94" s="13"/>
       <c r="C94" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>209</v>
@@ -4014,10 +4014,10 @@
         <v>13</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="57.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
       <c r="A95" s="16"/>
       <c r="B95" s="18" t="s">
         <v>111</v>
@@ -4044,7 +4044,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="71.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
       <c r="A96" s="16"/>
       <c r="B96" s="18"/>
       <c r="C96" s="14" t="s">
@@ -4066,10 +4066,10 @@
         <v>13</v>
       </c>
       <c r="I96" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="3" customFormat="1" ht="29.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="3" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
       <c r="A97" s="20"/>
       <c r="B97" s="21"/>
       <c r="C97" s="14" t="s">
@@ -4094,7 +4094,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
       <c r="A98" s="16"/>
       <c r="B98" s="18"/>
       <c r="C98" s="14" t="s">
@@ -4119,7 +4119,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="43.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:9" ht="45" thickTop="1" thickBot="1">
       <c r="A99" s="16"/>
       <c r="B99" s="18"/>
       <c r="C99" s="14" t="s">
@@ -4141,10 +4141,10 @@
         <v>13</v>
       </c>
       <c r="I99" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15.75" thickTop="1">
       <c r="B100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4152,35 +4152,35 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9">
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9">
       <c r="B105" s="2"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9">
       <c r="B106" s="2"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9">
       <c r="B107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9">
       <c r="B108" s="2"/>
     </row>
-    <row r="115" spans="16:26" x14ac:dyDescent="0.35">
+    <row r="115" spans="16:26">
       <c r="Y115" s="4"/>
     </row>
-    <row r="116" spans="16:26" x14ac:dyDescent="0.35">
+    <row r="116" spans="16:26">
       <c r="Z116" s="4"/>
     </row>
-    <row r="119" spans="16:26" x14ac:dyDescent="0.35">
+    <row r="119" spans="16:26">
       <c r="P119" s="4"/>
     </row>
-    <row r="120" spans="16:26" x14ac:dyDescent="0.35">
+    <row r="120" spans="16:26">
       <c r="P120" s="4"/>
       <c r="Q120" s="4"/>
     </row>
-    <row r="177" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="177" spans="16:16">
       <c r="P177" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add vplan item for future complete checking of lfsr lockup
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\work\ropeders\src\core-v-verif-secureseed\cv32e40s\docs\VerifPlans\Simulation\xsecure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E88BABB-1FF5-4068-BBD2-2FB75D0E6418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13D5CD-0A0C-4243-97B9-DD2C67349CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="29808" windowHeight="17496" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="346">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -1099,6 +1099,21 @@
   </si>
   <si>
     <t>A: a_xsecure_rf_ecc_gpr_not_all_0s_or_1s</t>
+  </si>
+  <si>
+    <t>LFSR Bad Seed</t>
+  </si>
+  <si>
+    <t>Certain seeds should eventually lead to the LFSR locking up. (This is different from explicitly writing it to 0 and causing an immediate lockup.)</t>
+  </si>
+  <si>
+    <t>Directed test</t>
+  </si>
+  <si>
+    <t>TODO:WARNING:silabs-robin</t>
+  </si>
+  <si>
+    <t>For all secureseed registers, write a value that eventually (but not immediately) leads to a lockup, and let the core run until that happens. (Could maybe be done with only a cover in formal, or with a simple directed test in sim, or both.)</t>
   </si>
 </sst>
 </file>
@@ -1628,30 +1643,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F85042D-12E0-4175-93E4-83EF6FCA4F4B}">
-  <dimension ref="A1:Z177"/>
+  <dimension ref="A1:Z178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="104.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="104.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1">
@@ -2314,7 +2329,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="43.5">
+    <row r="27" spans="1:9" ht="42">
       <c r="A27" s="16"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14" t="s">
@@ -2389,42 +2404,42 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="84" customHeight="1">
+    <row r="30" spans="1:9" ht="97.2">
       <c r="A30" s="16"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
-        <v>221</v>
+        <v>341</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>129</v>
+        <v>342</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>158</v>
+        <v>345</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>11</v>
+        <v>343</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="110.25" customHeight="1" thickBot="1">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="84" customHeight="1">
       <c r="A31" s="16"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14" t="s">
-        <v>131</v>
+        <v>221</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>233</v>
+        <v>129</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>11</v>
@@ -2436,22 +2451,20 @@
         <v>13</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="45" thickTop="1" thickBot="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="110.25" customHeight="1" thickBot="1">
       <c r="A32" s="16"/>
-      <c r="B32" s="18" t="s">
-        <v>75</v>
-      </c>
+      <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>79</v>
+        <v>233</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>11</v>
@@ -2460,186 +2473,190 @@
         <v>38</v>
       </c>
       <c r="H32" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
+      <c r="A33" s="16"/>
+      <c r="B33" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I33" s="12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="135.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="34" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
       <c r="A34" s="16"/>
       <c r="B34" s="18"/>
       <c r="C34" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>225</v>
+        <v>11</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>225</v>
+        <v>12</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>225</v>
+        <v>13</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="67.5" customHeight="1" thickTop="1" thickBot="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="135.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A35" s="16"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="14"/>
+      <c r="C35" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="D35" s="15" t="s">
-        <v>223</v>
+        <v>133</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>224</v>
+        <v>81</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>11</v>
+        <v>225</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="67.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="16"/>
       <c r="B36" s="18"/>
       <c r="C36" s="14"/>
       <c r="D36" s="15" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>139</v>
+        <v>224</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="G36" s="15" t="s">
         <v>38</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A37" s="16"/>
       <c r="B37" s="18"/>
       <c r="C37" s="14"/>
       <c r="D37" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>38</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="107.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A38" s="16"/>
       <c r="B38" s="18"/>
       <c r="C38" s="14"/>
       <c r="D38" s="15" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>302</v>
+        <v>59</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>38</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="81.75" customHeight="1" thickTop="1" thickBot="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="107.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A39" s="16"/>
       <c r="B39" s="18"/>
       <c r="C39" s="14"/>
       <c r="D39" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>78</v>
+        <v>302</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>38</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="48.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A40" s="12"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="81.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A40" s="16"/>
       <c r="B40" s="18"/>
       <c r="C40" s="14"/>
       <c r="D40" s="15" t="s">
-        <v>127</v>
+        <v>64</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F40" s="15" t="s">
         <v>11</v>
@@ -2651,18 +2668,18 @@
         <v>13</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="48.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A41" s="12"/>
       <c r="B41" s="18"/>
       <c r="C41" s="14"/>
       <c r="D41" s="15" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>11</v>
@@ -2674,20 +2691,18 @@
         <v>13</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="75" customHeight="1" thickTop="1" thickBot="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="50.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A42" s="12"/>
       <c r="B42" s="18"/>
-      <c r="C42" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="C42" s="14"/>
       <c r="D42" s="15" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>11</v>
@@ -2699,20 +2714,20 @@
         <v>13</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="110.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A43" s="16"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A43" s="12"/>
       <c r="B43" s="18"/>
       <c r="C43" s="14" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>11</v>
@@ -2724,20 +2739,20 @@
         <v>13</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="59.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="110.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="16"/>
       <c r="B44" s="18"/>
       <c r="C44" s="14" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>135</v>
+        <v>230</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>84</v>
+        <v>132</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>11</v>
@@ -2749,152 +2764,150 @@
         <v>13</v>
       </c>
       <c r="I44" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="59.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A45" s="16"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" thickTop="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="13" t="s">
+    <row r="46" spans="1:9" ht="28.8" thickTop="1">
+      <c r="A46" s="16"/>
+      <c r="B46" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C46" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D46" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E46" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H45" s="15" t="s">
+      <c r="H46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I45" s="12" t="s">
+      <c r="I46" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="86.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="72">
+    <row r="47" spans="1:9" ht="83.4">
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="F47" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="H47" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="60" customHeight="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="69.599999999999994">
       <c r="A48" s="16"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="132.75" customHeight="1" thickBot="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="60" customHeight="1">
       <c r="A49" s="16"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="132.75" customHeight="1" thickBot="1">
+      <c r="A50" s="16"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D50" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E50" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="F49" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="203.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A50" s="16"/>
-      <c r="B50" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>217</v>
-      </c>
       <c r="F50" s="15" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="G50" s="15" t="s">
         <v>235</v>
@@ -2903,141 +2916,143 @@
         <v>13</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="102.75" customHeight="1" thickTop="1" thickBot="1">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="203.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A51" s="16"/>
-      <c r="B51" s="18"/>
+      <c r="B51" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="C51" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>143</v>
+        <v>216</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>108</v>
+        <v>235</v>
       </c>
       <c r="H51" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="30.75" thickTop="1" thickBot="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="102.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A52" s="16"/>
       <c r="B52" s="18"/>
       <c r="C52" s="14" t="s">
-        <v>92</v>
+        <v>219</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="H52" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I52" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="200.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="29.4" thickTop="1" thickBot="1">
       <c r="A53" s="16"/>
       <c r="B53" s="18"/>
       <c r="C53" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="200.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A54" s="16"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D54" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E54" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="F53" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="15" t="s">
+      <c r="F54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H53" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="12" t="s">
+      <c r="H54" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="12" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="72.75" thickTop="1">
-      <c r="A54" s="16"/>
-      <c r="B54" s="13" t="s">
+    <row r="55" spans="1:10" ht="70.2" thickTop="1">
+      <c r="A55" s="16"/>
+      <c r="B55" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C55" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D55" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F55" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G54" s="15" t="s">
+      <c r="G55" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H55" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I54" s="12" t="s">
+      <c r="I55" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="57.75">
-      <c r="A55" s="16"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="57.75">
+    <row r="56" spans="1:10" ht="42">
       <c r="A56" s="16"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>303</v>
@@ -3055,14 +3070,14 @@
         <v>13</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="57.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="42">
       <c r="A57" s="16"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>303</v>
@@ -3080,14 +3095,14 @@
         <v>13</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="57.75">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="42">
       <c r="A58" s="16"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D58" s="15" t="s">
         <v>303</v>
@@ -3105,15 +3120,14 @@
         <v>13</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="J58" s="15"/>
-    </row>
-    <row r="59" spans="1:11" ht="57.75">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="42">
       <c r="A59" s="16"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>303</v>
@@ -3131,14 +3145,15 @@
         <v>13</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="57.75">
+        <v>339</v>
+      </c>
+      <c r="J59" s="15"/>
+    </row>
+    <row r="60" spans="1:10" ht="42">
       <c r="A60" s="16"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>303</v>
@@ -3156,14 +3171,14 @@
         <v>13</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="57.75">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="42">
       <c r="A61" s="16"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>303</v>
@@ -3181,14 +3196,14 @@
         <v>13</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="57.75">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="42">
       <c r="A62" s="16"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D62" s="15" t="s">
         <v>303</v>
@@ -3206,14 +3221,14 @@
         <v>13</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="57.75">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="42">
       <c r="A63" s="16"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>303</v>
@@ -3231,14 +3246,14 @@
         <v>13</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="57.75">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="42">
       <c r="A64" s="16"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>303</v>
@@ -3258,13 +3273,12 @@
       <c r="I64" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="K64" s="15"/>
-    </row>
-    <row r="65" spans="1:11" ht="57.75">
+    </row>
+    <row r="65" spans="1:11" ht="42">
       <c r="A65" s="16"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>303</v>
@@ -3286,11 +3300,11 @@
       </c>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" ht="57.75">
+    <row r="66" spans="1:11" ht="42">
       <c r="A66" s="16"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="D66" s="15" t="s">
         <v>303</v>
@@ -3308,14 +3322,15 @@
         <v>13</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="57.75">
+        <v>330</v>
+      </c>
+      <c r="K66" s="15"/>
+    </row>
+    <row r="67" spans="1:11" ht="42">
       <c r="A67" s="16"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>303</v>
@@ -3333,14 +3348,14 @@
         <v>13</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="57.75">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="42">
       <c r="A68" s="16"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>303</v>
@@ -3358,14 +3373,14 @@
         <v>13</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="57.75">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="42">
       <c r="A69" s="16"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D69" s="15" t="s">
         <v>303</v>
@@ -3383,14 +3398,14 @@
         <v>13</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="57.75">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="42">
       <c r="A70" s="16"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>303</v>
@@ -3408,14 +3423,14 @@
         <v>13</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="57.75">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="42">
       <c r="A71" s="16"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D71" s="15" t="s">
         <v>303</v>
@@ -3433,14 +3448,14 @@
         <v>13</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="57.75">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="42">
       <c r="A72" s="16"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>303</v>
@@ -3458,14 +3473,14 @@
         <v>13</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="58.5" thickBot="1">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="42">
       <c r="A73" s="16"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>303</v>
@@ -3483,97 +3498,97 @@
         <v>13</v>
       </c>
       <c r="I73" s="12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="42.6" thickBot="1">
+      <c r="A74" s="16"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="12" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A74" s="12"/>
-      <c r="B74" s="18" t="s">
+    <row r="75" spans="1:11" s="1" customFormat="1" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A75" s="12"/>
+      <c r="B75" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C75" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D75" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E75" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="F74" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G74" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="H74" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I74" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
-      <c r="A75" s="12"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="F75" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="H75" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I75" s="16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" ht="45" thickTop="1" thickBot="1">
+      <c r="I75" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="1" customFormat="1" ht="29.4" thickTop="1" thickBot="1">
       <c r="A76" s="12"/>
       <c r="B76" s="18"/>
       <c r="C76" s="14" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F76" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H76" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
       <c r="A77" s="12"/>
       <c r="B77" s="18"/>
       <c r="C77" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="F77" s="15" t="s">
         <v>120</v>
@@ -3585,20 +3600,20 @@
         <v>13</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
       <c r="A78" s="12"/>
       <c r="B78" s="18"/>
       <c r="C78" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="F78" s="15" t="s">
         <v>120</v>
@@ -3610,20 +3625,20 @@
         <v>13</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
       <c r="A79" s="12"/>
       <c r="B79" s="18"/>
       <c r="C79" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F79" s="15" t="s">
         <v>120</v>
@@ -3635,45 +3650,45 @@
         <v>13</v>
       </c>
       <c r="I79" s="16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
       <c r="A80" s="12"/>
       <c r="B80" s="18"/>
-      <c r="C80" s="16" t="s">
-        <v>180</v>
+      <c r="C80" s="14" t="s">
+        <v>172</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>288</v>
+        <v>173</v>
       </c>
       <c r="F80" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="H80" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I80" s="12" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" s="1" customFormat="1" ht="101.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="I80" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="1" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A81" s="12"/>
       <c r="B81" s="18"/>
-      <c r="C81" s="14" t="s">
-        <v>181</v>
+      <c r="C81" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>175</v>
+        <v>288</v>
       </c>
       <c r="F81" s="15" t="s">
         <v>120</v>
@@ -3685,23 +3700,23 @@
         <v>13</v>
       </c>
       <c r="I81" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="1" customFormat="1" ht="102" thickTop="1" thickBot="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="1" customFormat="1" ht="101.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A82" s="12"/>
       <c r="B82" s="18"/>
       <c r="C82" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="G82" s="15" t="s">
         <v>108</v>
@@ -3709,24 +3724,24 @@
       <c r="H82" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I82" s="16" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="1" customFormat="1" ht="164.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="I82" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="1" customFormat="1" ht="84.6" thickTop="1" thickBot="1">
       <c r="A83" s="12"/>
       <c r="B83" s="18"/>
       <c r="C83" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>108</v>
@@ -3734,24 +3749,24 @@
       <c r="H83" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+      <c r="I83" s="16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="1" customFormat="1" ht="164.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A84" s="12"/>
       <c r="B84" s="18"/>
-      <c r="C84" s="16" t="s">
-        <v>147</v>
+      <c r="C84" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>108</v>
@@ -3760,20 +3775,20 @@
         <v>13</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1" thickBot="1">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="1" customFormat="1" ht="70.8" thickTop="1" thickBot="1">
       <c r="A85" s="12"/>
       <c r="B85" s="18"/>
       <c r="C85" s="16" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="D85" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F85" s="15" t="s">
         <v>11</v>
@@ -3785,20 +3800,20 @@
         <v>13</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A86" s="12"/>
       <c r="B86" s="18"/>
       <c r="C86" s="16" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D86" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>253</v>
+        <v>188</v>
       </c>
       <c r="F86" s="15" t="s">
         <v>11</v>
@@ -3810,20 +3825,20 @@
         <v>13</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
       <c r="A87" s="12"/>
       <c r="B87" s="18"/>
       <c r="C87" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>191</v>
+        <v>253</v>
       </c>
       <c r="F87" s="15" t="s">
         <v>11</v>
@@ -3835,20 +3850,20 @@
         <v>13</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
       <c r="A88" s="12"/>
       <c r="B88" s="18"/>
       <c r="C88" s="16" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F88" s="15" t="s">
         <v>11</v>
@@ -3860,20 +3875,20 @@
         <v>13</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="1" customFormat="1" ht="93" customHeight="1" thickTop="1" thickBot="1">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="1" customFormat="1" ht="70.8" thickTop="1" thickBot="1">
       <c r="A89" s="12"/>
       <c r="B89" s="18"/>
       <c r="C89" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F89" s="15" t="s">
         <v>11</v>
@@ -3882,44 +3897,44 @@
         <v>108</v>
       </c>
       <c r="H89" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="1" customFormat="1" ht="93" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A90" s="12"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H90" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I89" s="12" t="s">
+      <c r="I90" s="12" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="98.25" customHeight="1" thickTop="1">
-      <c r="A90" s="16"/>
-      <c r="B90" s="13" t="s">
+    <row r="91" spans="1:9" ht="98.25" customHeight="1" thickTop="1">
+      <c r="A91" s="16"/>
+      <c r="B91" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C91" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E90" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="F90" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="H90" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I90" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="96.75" customHeight="1">
-      <c r="A91" s="16"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="14" t="s">
-        <v>206</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>204</v>
@@ -3937,16 +3952,14 @@
         <v>13</v>
       </c>
       <c r="I91" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="95.25" customHeight="1">
-      <c r="A92" s="16" t="s">
-        <v>203</v>
-      </c>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="96.75" customHeight="1">
+      <c r="A92" s="16"/>
       <c r="B92" s="13"/>
       <c r="C92" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>204</v>
@@ -3964,20 +3977,22 @@
         <v>13</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="99" customHeight="1">
-      <c r="A93" s="16"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="95.25" customHeight="1">
+      <c r="A93" s="16" t="s">
+        <v>203</v>
+      </c>
       <c r="B93" s="13"/>
       <c r="C93" s="14" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E93" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F93" s="15" t="s">
         <v>11</v>
@@ -3989,14 +4004,14 @@
         <v>13</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="81" customHeight="1" thickBot="1">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="99" customHeight="1">
       <c r="A94" s="16"/>
       <c r="B94" s="13"/>
       <c r="C94" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D94" s="15" t="s">
         <v>209</v>
@@ -4014,97 +4029,97 @@
         <v>13</v>
       </c>
       <c r="I94" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="81" customHeight="1" thickBot="1">
+      <c r="A95" s="16"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G95" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H95" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I95" s="12" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
-      <c r="A95" s="16"/>
-      <c r="B95" s="18" t="s">
+    <row r="96" spans="1:9" ht="43.2" thickTop="1" thickBot="1">
+      <c r="A96" s="16"/>
+      <c r="B96" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C96" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D96" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E95" s="15" t="s">
+      <c r="E96" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F96" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G95" s="15" t="s">
+      <c r="G96" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H95" s="15" t="s">
+      <c r="H96" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I95" s="12" t="s">
+      <c r="I96" s="12" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
-      <c r="A96" s="16"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="14" t="s">
+    <row r="97" spans="1:9" ht="57" thickTop="1" thickBot="1">
+      <c r="A97" s="16"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="D97" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E96" s="15" t="s">
+      <c r="E97" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F96" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G96" s="15" t="s">
+      <c r="F97" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H96" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I96" s="12" t="s">
+      <c r="H97" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="3" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
-      <c r="A97" s="20"/>
-      <c r="B97" s="21"/>
-      <c r="C97" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E97" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G97" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I97" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
-      <c r="A98" s="16"/>
-      <c r="B98" s="18"/>
+    <row r="98" spans="1:9" s="3" customFormat="1" ht="29.4" thickTop="1" thickBot="1">
+      <c r="A98" s="20"/>
+      <c r="B98" s="21"/>
       <c r="C98" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E98" s="15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F98" s="15" t="s">
         <v>44</v>
@@ -4119,41 +4134,63 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="45" thickTop="1" thickBot="1">
+    <row r="99" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
       <c r="A99" s="16"/>
       <c r="B99" s="18"/>
       <c r="C99" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E99" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F99" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G99" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H99" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="43.2" thickTop="1" thickBot="1">
+      <c r="A100" s="16"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="D99" s="15" t="s">
+      <c r="D100" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="E99" s="15" t="s">
+      <c r="E100" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="F99" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G99" s="15" t="s">
+      <c r="F100" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H99" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I99" s="12" t="s">
+      <c r="H100" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I100" s="12" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="15.75" thickTop="1">
-      <c r="B100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="B104" s="2"/>
+    <row r="101" spans="1:9" ht="15" thickTop="1">
+      <c r="B101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
     </row>
     <row r="105" spans="1:9">
       <c r="B105" s="2"/>
@@ -4167,21 +4204,24 @@
     <row r="108" spans="1:9">
       <c r="B108" s="2"/>
     </row>
-    <row r="115" spans="16:26">
-      <c r="Y115" s="4"/>
+    <row r="109" spans="1:9">
+      <c r="B109" s="2"/>
     </row>
     <row r="116" spans="16:26">
-      <c r="Z116" s="4"/>
-    </row>
-    <row r="119" spans="16:26">
-      <c r="P119" s="4"/>
+      <c r="Y116" s="4"/>
+    </row>
+    <row r="117" spans="16:26">
+      <c r="Z117" s="4"/>
     </row>
     <row r="120" spans="16:26">
       <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-    </row>
-    <row r="177" spans="16:16">
-      <c r="P177" s="4"/>
+    </row>
+    <row r="121" spans="16:26">
+      <c r="P121" s="4"/>
+      <c r="Q121" s="4"/>
+    </row>
+    <row r="178" spans="16:16">
+      <c r="P178" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correct xsecure coverage property items
Signed-off-by: Kristine Dosvik <krdosvik@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/xsecure/xsecure_vplan.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\work\ropeders\src\core-v-verif-secureseed\cv32e40s\docs\VerifPlans\Simulation\xsecure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krdosvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13D5CD-0A0C-4243-97B9-DD2C67349CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFD7E53-4977-46AC-A090-3D805B43DAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-108" windowWidth="29808" windowHeight="17496" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{209BFBE4-008D-4F8A-8F6D-9E555E6ABA2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -900,9 +900,6 @@
     <t>A: a_xsecure_hint_instr_load_hint_stall</t>
   </si>
   <si>
-    <t>A: a_glitch_xsecure_integrity_data_integrity_err_helper_assert, a_glitch_xsecure_integrity_data_integrity_err. COV:c_glitch_xsecure_security_parity_checksum_fault_NMI_load_instruction, c_glitch_xsecure_security_parity_checksum_fault_NMI_store_instruction</t>
-  </si>
-  <si>
     <t>A: a_glitch_xsecure_integrity_instr_integrity_error</t>
   </si>
   <si>
@@ -1114,6 +1111,9 @@
   </si>
   <si>
     <t>For all secureseed registers, write a value that eventually (but not immediately) leads to a lockup, and let the core run until that happens. (Could maybe be done with only a cover in formal, or with a simple directed test in sim, or both.)</t>
+  </si>
+  <si>
+    <t>A: a_glitch_xsecure_integrity_data_integrity_err_helper_assert, a_glitch_xsecure_integrity_data_integrity_err. COV:c_glitch_xsecure_integrity_parity_checksum_fault_NMI_load_instruction, c_glitch_xsecure_integrity_parity_checksum_fault_NMI_store_instruction.</t>
   </si>
 </sst>
 </file>
@@ -1646,27 +1646,27 @@
   <dimension ref="A1:Z178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="104.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="104.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="14.5546875" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" customWidth="1"/>
-    <col min="18" max="18" width="17.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="6" customFormat="1">
@@ -1700,7 +1700,7 @@
     </row>
     <row r="2" spans="1:9" ht="238.5" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>9</v>
@@ -2039,7 +2039,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>60</v>
@@ -2051,7 +2051,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="48" customHeight="1">
@@ -2139,7 +2139,7 @@
         <v>57</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>60</v>
@@ -2151,7 +2151,7 @@
         <v>36</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="77.25" customHeight="1">
@@ -2189,7 +2189,7 @@
         <v>61</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>60</v>
@@ -2201,7 +2201,7 @@
         <v>36</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="81.75" customHeight="1">
@@ -2329,7 +2329,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="42">
+    <row r="27" spans="1:9" ht="43.5">
       <c r="A27" s="16"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14" t="s">
@@ -2351,7 +2351,7 @@
         <v>36</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="54" customHeight="1">
@@ -2404,20 +2404,20 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="97.2">
+    <row r="30" spans="1:9" ht="100.5">
       <c r="A30" s="16"/>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="E30" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>342</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>343</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>45</v>
@@ -2426,7 +2426,7 @@
         <v>37</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="84" customHeight="1">
@@ -2479,7 +2479,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
+    <row r="33" spans="1:9" ht="45" thickTop="1" thickBot="1">
       <c r="A33" s="16"/>
       <c r="B33" s="18" t="s">
         <v>75</v>
@@ -2506,7 +2506,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
+    <row r="34" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
       <c r="A34" s="16"/>
       <c r="B34" s="18"/>
       <c r="C34" s="14" t="s">
@@ -2599,7 +2599,7 @@
         <v>36</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="77.25" customHeight="1" thickTop="1" thickBot="1">
@@ -2633,7 +2633,7 @@
         <v>61</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F39" s="15" t="s">
         <v>60</v>
@@ -2645,7 +2645,7 @@
         <v>37</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="81.75" customHeight="1" thickTop="1" thickBot="1">
@@ -2792,7 +2792,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="28.8" thickTop="1">
+    <row r="46" spans="1:9" ht="30" thickTop="1">
       <c r="A46" s="16"/>
       <c r="B46" s="13" t="s">
         <v>85</v>
@@ -2819,7 +2819,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="83.4">
+    <row r="47" spans="1:9" ht="86.25">
       <c r="A47" s="16"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14" t="s">
@@ -2844,7 +2844,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="69.599999999999994">
+    <row r="48" spans="1:9" ht="72">
       <c r="A48" s="16"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14" t="s">
@@ -2916,7 +2916,7 @@
         <v>13</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="203.25" customHeight="1" thickTop="1" thickBot="1">
@@ -2971,7 +2971,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="29.4" thickTop="1" thickBot="1">
+    <row r="53" spans="1:10" ht="30.75" thickTop="1" thickBot="1">
       <c r="A53" s="16"/>
       <c r="B53" s="18"/>
       <c r="C53" s="14" t="s">
@@ -3021,7 +3021,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="70.2" thickTop="1">
+    <row r="55" spans="1:10" ht="72.75" thickTop="1">
       <c r="A55" s="16"/>
       <c r="B55" s="13" t="s">
         <v>94</v>
@@ -3048,17 +3048,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="42">
+    <row r="56" spans="1:10" ht="57.75">
       <c r="A56" s="16"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F56" s="15" t="s">
         <v>11</v>
@@ -3070,20 +3070,20 @@
         <v>13</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="42">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="57.75">
       <c r="A57" s="16"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F57" s="15" t="s">
         <v>11</v>
@@ -3095,20 +3095,20 @@
         <v>13</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="42">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="57.75">
       <c r="A58" s="16"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>11</v>
@@ -3120,20 +3120,20 @@
         <v>13</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="42">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="57.75">
       <c r="A59" s="16"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F59" s="15" t="s">
         <v>11</v>
@@ -3145,21 +3145,21 @@
         <v>13</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J59" s="15"/>
     </row>
-    <row r="60" spans="1:10" ht="42">
+    <row r="60" spans="1:10" ht="57.75">
       <c r="A60" s="16"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F60" s="15" t="s">
         <v>11</v>
@@ -3171,20 +3171,20 @@
         <v>13</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="42">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="57.75">
       <c r="A61" s="16"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F61" s="15" t="s">
         <v>11</v>
@@ -3196,20 +3196,20 @@
         <v>13</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="42">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="57.75">
       <c r="A62" s="16"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F62" s="15" t="s">
         <v>11</v>
@@ -3221,20 +3221,20 @@
         <v>13</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="42">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="57.75">
       <c r="A63" s="16"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>11</v>
@@ -3246,20 +3246,20 @@
         <v>13</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="42">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="57.75">
       <c r="A64" s="16"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>11</v>
@@ -3271,20 +3271,20 @@
         <v>13</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="42">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="57.75">
       <c r="A65" s="16"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>11</v>
@@ -3296,21 +3296,21 @@
         <v>13</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" ht="42">
+    <row r="66" spans="1:11" ht="57.75">
       <c r="A66" s="16"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>11</v>
@@ -3322,21 +3322,21 @@
         <v>13</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" ht="42">
+    <row r="67" spans="1:11" ht="57.75">
       <c r="A67" s="16"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>11</v>
@@ -3348,20 +3348,20 @@
         <v>13</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="42">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="57.75">
       <c r="A68" s="16"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F68" s="15" t="s">
         <v>11</v>
@@ -3373,20 +3373,20 @@
         <v>13</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="42">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="57.75">
       <c r="A69" s="16"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F69" s="15" t="s">
         <v>11</v>
@@ -3398,20 +3398,20 @@
         <v>13</v>
       </c>
       <c r="I69" s="12" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="42">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="57.75">
       <c r="A70" s="16"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F70" s="15" t="s">
         <v>11</v>
@@ -3423,20 +3423,20 @@
         <v>13</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="42">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="57.75">
       <c r="A71" s="16"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F71" s="15" t="s">
         <v>11</v>
@@ -3448,20 +3448,20 @@
         <v>13</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="42">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="57.75">
       <c r="A72" s="16"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>11</v>
@@ -3473,20 +3473,20 @@
         <v>13</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="42">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="57.75">
       <c r="A73" s="16"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>11</v>
@@ -3498,20 +3498,20 @@
         <v>13</v>
       </c>
       <c r="I73" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="42.6" thickBot="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="58.5" thickBot="1">
       <c r="A74" s="16"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F74" s="15" t="s">
         <v>11</v>
@@ -3523,7 +3523,7 @@
         <v>13</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="1" customFormat="1" ht="108.75" customHeight="1" thickTop="1" thickBot="1">
@@ -3550,10 +3550,10 @@
         <v>13</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" ht="29.4" thickTop="1" thickBot="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="1" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
       <c r="A76" s="12"/>
       <c r="B76" s="18"/>
       <c r="C76" s="14" t="s">
@@ -3578,7 +3578,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="45" thickTop="1" thickBot="1">
       <c r="A77" s="12"/>
       <c r="B77" s="18"/>
       <c r="C77" s="14" t="s">
@@ -3603,7 +3603,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A78" s="12"/>
       <c r="B78" s="18"/>
       <c r="C78" s="14" t="s">
@@ -3628,7 +3628,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
+    <row r="79" spans="1:11" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A79" s="12"/>
       <c r="B79" s="18"/>
       <c r="C79" s="14" t="s">
@@ -3653,7 +3653,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" ht="57" thickTop="1" thickBot="1">
+    <row r="80" spans="1:11" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A80" s="12"/>
       <c r="B80" s="18"/>
       <c r="C80" s="14" t="s">
@@ -3688,7 +3688,7 @@
         <v>176</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F81" s="15" t="s">
         <v>120</v>
@@ -3700,7 +3700,7 @@
         <v>13</v>
       </c>
       <c r="I81" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="1" customFormat="1" ht="101.25" customHeight="1" thickTop="1" thickBot="1">
@@ -3725,10 +3725,10 @@
         <v>13</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="1" customFormat="1" ht="84.6" thickTop="1" thickBot="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="1" customFormat="1" ht="102" thickTop="1" thickBot="1">
       <c r="A83" s="12"/>
       <c r="B83" s="18"/>
       <c r="C83" s="14" t="s">
@@ -3750,7 +3750,7 @@
         <v>13</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="1" customFormat="1" ht="164.25" customHeight="1" thickTop="1" thickBot="1">
@@ -3775,10 +3775,10 @@
         <v>13</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="1" customFormat="1" ht="70.8" thickTop="1" thickBot="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A85" s="12"/>
       <c r="B85" s="18"/>
       <c r="C85" s="16" t="s">
@@ -3800,7 +3800,7 @@
         <v>13</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="1" customFormat="1" ht="94.5" customHeight="1" thickTop="1" thickBot="1">
@@ -3825,10 +3825,10 @@
         <v>13</v>
       </c>
       <c r="I86" s="12" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A87" s="12"/>
       <c r="B87" s="18"/>
       <c r="C87" s="16" t="s">
@@ -3850,10 +3850,10 @@
         <v>13</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="1" customFormat="1" ht="43.2" thickTop="1" thickBot="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="1" customFormat="1" ht="59.25" thickTop="1" thickBot="1">
       <c r="A88" s="12"/>
       <c r="B88" s="18"/>
       <c r="C88" s="16" t="s">
@@ -3875,10 +3875,10 @@
         <v>13</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="1" customFormat="1" ht="70.8" thickTop="1" thickBot="1">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="1" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A89" s="12"/>
       <c r="B89" s="18"/>
       <c r="C89" s="16" t="s">
@@ -3900,7 +3900,7 @@
         <v>13</v>
       </c>
       <c r="I89" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="1" customFormat="1" ht="93" customHeight="1" thickTop="1" thickBot="1">
@@ -3925,7 +3925,7 @@
         <v>37</v>
       </c>
       <c r="I90" s="12" t="s">
-        <v>281</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="98.25" customHeight="1" thickTop="1">
@@ -4057,7 +4057,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="43.2" thickTop="1" thickBot="1">
+    <row r="96" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
       <c r="A96" s="16"/>
       <c r="B96" s="18" t="s">
         <v>111</v>
@@ -4084,7 +4084,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="57" thickTop="1" thickBot="1">
+    <row r="97" spans="1:9" ht="59.25" thickTop="1" thickBot="1">
       <c r="A97" s="16"/>
       <c r="B97" s="18"/>
       <c r="C97" s="14" t="s">
@@ -4109,7 +4109,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="3" customFormat="1" ht="29.4" thickTop="1" thickBot="1">
+    <row r="98" spans="1:9" s="3" customFormat="1" ht="30.75" thickTop="1" thickBot="1">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="14" t="s">
@@ -4134,7 +4134,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="29.4" thickTop="1" thickBot="1">
+    <row r="99" spans="1:9" ht="30.75" thickTop="1" thickBot="1">
       <c r="A99" s="16"/>
       <c r="B99" s="18"/>
       <c r="C99" s="14" t="s">
@@ -4159,7 +4159,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="43.2" thickTop="1" thickBot="1">
+    <row r="100" spans="1:9" ht="45" thickTop="1" thickBot="1">
       <c r="A100" s="16"/>
       <c r="B100" s="18"/>
       <c r="C100" s="14" t="s">
@@ -4184,7 +4184,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="15" thickTop="1">
+    <row r="101" spans="1:9" ht="15.75" thickTop="1">
       <c r="B101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>

</xml_diff>